<commit_message>
Se quitó COB Acapulco
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -2265,7 +2265,7 @@
         <v>90</v>
       </c>
       <c r="D77">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E77">
         <v>124</v>
@@ -2299,7 +2299,7 @@
         <v>92</v>
       </c>
       <c r="D79">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E79">
         <v>209</v>
@@ -2316,7 +2316,7 @@
         <v>93</v>
       </c>
       <c r="D80">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E80">
         <v>221</v>
@@ -2350,7 +2350,7 @@
         <v>95</v>
       </c>
       <c r="D82">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E82">
         <v>343</v>
@@ -2367,7 +2367,7 @@
         <v>96</v>
       </c>
       <c r="D83">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E83">
         <v>335</v>
@@ -2384,7 +2384,7 @@
         <v>97</v>
       </c>
       <c r="D84">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E84">
         <v>410</v>
@@ -2401,7 +2401,7 @@
         <v>98</v>
       </c>
       <c r="D85">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E85">
         <v>334</v>
@@ -2435,7 +2435,7 @@
         <v>100</v>
       </c>
       <c r="D87">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E87">
         <v>166</v>
@@ -2469,7 +2469,7 @@
         <v>102</v>
       </c>
       <c r="D89">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E89">
         <v>94</v>
@@ -2486,7 +2486,7 @@
         <v>103</v>
       </c>
       <c r="D90">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E90">
         <v>138</v>
@@ -2503,7 +2503,7 @@
         <v>104</v>
       </c>
       <c r="D91">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E91">
         <v>155</v>
@@ -2520,7 +2520,7 @@
         <v>105</v>
       </c>
       <c r="D92">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E92">
         <v>92</v>
@@ -2537,7 +2537,7 @@
         <v>106</v>
       </c>
       <c r="D93">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E93">
         <v>84</v>
@@ -2571,7 +2571,7 @@
         <v>108</v>
       </c>
       <c r="D95">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E95">
         <v>121</v>
@@ -2622,7 +2622,7 @@
         <v>111</v>
       </c>
       <c r="D98">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E98">
         <v>175</v>
@@ -2639,7 +2639,7 @@
         <v>112</v>
       </c>
       <c r="D99">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E99">
         <v>136</v>
@@ -2656,7 +2656,7 @@
         <v>113</v>
       </c>
       <c r="D100">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E100">
         <v>261</v>
@@ -2673,7 +2673,7 @@
         <v>114</v>
       </c>
       <c r="D101">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E101">
         <v>170</v>
@@ -2690,7 +2690,7 @@
         <v>115</v>
       </c>
       <c r="D102">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E102">
         <v>171</v>
@@ -2707,7 +2707,7 @@
         <v>116</v>
       </c>
       <c r="D103">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E103">
         <v>230</v>
@@ -2724,7 +2724,7 @@
         <v>117</v>
       </c>
       <c r="D104">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E104">
         <v>277</v>
@@ -2741,7 +2741,7 @@
         <v>118</v>
       </c>
       <c r="D105">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E105">
         <v>280</v>
@@ -2775,7 +2775,7 @@
         <v>120</v>
       </c>
       <c r="D107">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E107">
         <v>277</v>
@@ -2792,7 +2792,7 @@
         <v>121</v>
       </c>
       <c r="D108">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E108">
         <v>139</v>
@@ -2809,7 +2809,7 @@
         <v>122</v>
       </c>
       <c r="D109">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E109">
         <v>164</v>
@@ -2826,7 +2826,7 @@
         <v>123</v>
       </c>
       <c r="D110">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E110">
         <v>154</v>
@@ -2877,7 +2877,7 @@
         <v>126</v>
       </c>
       <c r="D113">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E113">
         <v>149</v>
@@ -2962,7 +2962,7 @@
         <v>131</v>
       </c>
       <c r="D118">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E118">
         <v>355</v>
@@ -3013,7 +3013,7 @@
         <v>134</v>
       </c>
       <c r="D121">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E121">
         <v>124</v>
@@ -3030,7 +3030,7 @@
         <v>135</v>
       </c>
       <c r="D122">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E122">
         <v>142</v>
@@ -3047,7 +3047,7 @@
         <v>136</v>
       </c>
       <c r="D123">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E123">
         <v>305</v>
@@ -3081,7 +3081,7 @@
         <v>138</v>
       </c>
       <c r="D125">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E125">
         <v>197</v>
@@ -3115,7 +3115,7 @@
         <v>140</v>
       </c>
       <c r="D127">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E127">
         <v>153</v>
@@ -3183,7 +3183,7 @@
         <v>144</v>
       </c>
       <c r="D131">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E131">
         <v>248</v>
@@ -3798,7 +3798,7 @@
         <v>18</v>
       </c>
       <c r="E167">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3815,7 +3815,7 @@
         <v>11</v>
       </c>
       <c r="E168">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3832,7 +3832,7 @@
         <v>21</v>
       </c>
       <c r="E169">
-        <v>190</v>
+        <v>236</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3849,7 +3849,7 @@
         <v>27</v>
       </c>
       <c r="E170">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3866,7 +3866,7 @@
         <v>21</v>
       </c>
       <c r="E171">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3883,7 +3883,7 @@
         <v>21</v>
       </c>
       <c r="E172">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4033,10 +4033,10 @@
         <v>194</v>
       </c>
       <c r="D181">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E181">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5223,7 +5223,7 @@
         <v>84</v>
       </c>
       <c r="D251">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E251">
         <v>119</v>
@@ -5240,7 +5240,7 @@
         <v>85</v>
       </c>
       <c r="D252">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E252">
         <v>71</v>
@@ -5257,7 +5257,7 @@
         <v>86</v>
       </c>
       <c r="D253">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E253">
         <v>61</v>
@@ -5274,7 +5274,7 @@
         <v>87</v>
       </c>
       <c r="D254">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E254">
         <v>65</v>
@@ -5308,7 +5308,7 @@
         <v>89</v>
       </c>
       <c r="D256">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E256">
         <v>65</v>
@@ -5359,7 +5359,7 @@
         <v>92</v>
       </c>
       <c r="D259">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E259">
         <v>76</v>
@@ -5376,7 +5376,7 @@
         <v>93</v>
       </c>
       <c r="D260">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E260">
         <v>53</v>
@@ -5393,7 +5393,7 @@
         <v>94</v>
       </c>
       <c r="D261">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E261">
         <v>55</v>
@@ -5410,7 +5410,7 @@
         <v>95</v>
       </c>
       <c r="D262">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E262">
         <v>102</v>
@@ -5427,7 +5427,7 @@
         <v>96</v>
       </c>
       <c r="D263">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E263">
         <v>142</v>
@@ -5444,7 +5444,7 @@
         <v>97</v>
       </c>
       <c r="D264">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E264">
         <v>166</v>
@@ -5512,7 +5512,7 @@
         <v>101</v>
       </c>
       <c r="D268">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E268">
         <v>43</v>
@@ -5529,7 +5529,7 @@
         <v>102</v>
       </c>
       <c r="D269">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E269">
         <v>31</v>
@@ -5546,7 +5546,7 @@
         <v>103</v>
       </c>
       <c r="D270">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E270">
         <v>26</v>
@@ -5563,7 +5563,7 @@
         <v>104</v>
       </c>
       <c r="D271">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E271">
         <v>36</v>
@@ -5580,7 +5580,7 @@
         <v>105</v>
       </c>
       <c r="D272">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E272">
         <v>34</v>
@@ -5614,7 +5614,7 @@
         <v>107</v>
       </c>
       <c r="D274">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E274">
         <v>41</v>
@@ -5631,7 +5631,7 @@
         <v>108</v>
       </c>
       <c r="D275">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E275">
         <v>47</v>
@@ -5648,7 +5648,7 @@
         <v>109</v>
       </c>
       <c r="D276">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E276">
         <v>53</v>
@@ -5665,7 +5665,7 @@
         <v>110</v>
       </c>
       <c r="D277">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E277">
         <v>73</v>
@@ -5682,7 +5682,7 @@
         <v>111</v>
       </c>
       <c r="D278">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E278">
         <v>96</v>
@@ -5699,7 +5699,7 @@
         <v>112</v>
       </c>
       <c r="D279">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E279">
         <v>58</v>
@@ -5733,7 +5733,7 @@
         <v>114</v>
       </c>
       <c r="D281">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E281">
         <v>68</v>
@@ -5750,7 +5750,7 @@
         <v>115</v>
       </c>
       <c r="D282">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E282">
         <v>60</v>
@@ -5767,7 +5767,7 @@
         <v>116</v>
       </c>
       <c r="D283">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E283">
         <v>76</v>
@@ -5784,7 +5784,7 @@
         <v>117</v>
       </c>
       <c r="D284">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E284">
         <v>84</v>
@@ -5801,7 +5801,7 @@
         <v>118</v>
       </c>
       <c r="D285">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E285">
         <v>202</v>
@@ -5818,7 +5818,7 @@
         <v>119</v>
       </c>
       <c r="D286">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E286">
         <v>209</v>
@@ -5835,7 +5835,7 @@
         <v>120</v>
       </c>
       <c r="D287">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E287">
         <v>115</v>
@@ -5852,7 +5852,7 @@
         <v>121</v>
       </c>
       <c r="D288">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E288">
         <v>50</v>
@@ -5869,7 +5869,7 @@
         <v>122</v>
       </c>
       <c r="D289">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E289">
         <v>61</v>
@@ -5886,7 +5886,7 @@
         <v>123</v>
       </c>
       <c r="D290">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E290">
         <v>64</v>
@@ -5903,7 +5903,7 @@
         <v>124</v>
       </c>
       <c r="D291">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E291">
         <v>113</v>
@@ -5920,7 +5920,7 @@
         <v>125</v>
       </c>
       <c r="D292">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E292">
         <v>62</v>
@@ -5937,7 +5937,7 @@
         <v>126</v>
       </c>
       <c r="D293">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E293">
         <v>65</v>
@@ -5954,7 +5954,7 @@
         <v>127</v>
       </c>
       <c r="D294">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E294">
         <v>69</v>
@@ -5971,7 +5971,7 @@
         <v>128</v>
       </c>
       <c r="D295">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E295">
         <v>56</v>
@@ -5988,7 +5988,7 @@
         <v>129</v>
       </c>
       <c r="D296">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E296">
         <v>69</v>
@@ -6005,7 +6005,7 @@
         <v>130</v>
       </c>
       <c r="D297">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E297">
         <v>116</v>
@@ -6022,7 +6022,7 @@
         <v>131</v>
       </c>
       <c r="D298">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E298">
         <v>160</v>
@@ -6039,7 +6039,7 @@
         <v>132</v>
       </c>
       <c r="D299">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E299">
         <v>199</v>
@@ -6073,7 +6073,7 @@
         <v>134</v>
       </c>
       <c r="D301">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E301">
         <v>43</v>
@@ -6090,7 +6090,7 @@
         <v>135</v>
       </c>
       <c r="D302">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E302">
         <v>58</v>
@@ -6107,7 +6107,7 @@
         <v>136</v>
       </c>
       <c r="D303">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E303">
         <v>94</v>
@@ -6124,7 +6124,7 @@
         <v>137</v>
       </c>
       <c r="D304">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E304">
         <v>52</v>
@@ -6141,7 +6141,7 @@
         <v>138</v>
       </c>
       <c r="D305">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E305">
         <v>74</v>
@@ -6158,7 +6158,7 @@
         <v>139</v>
       </c>
       <c r="D306">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E306">
         <v>60</v>
@@ -6175,7 +6175,7 @@
         <v>140</v>
       </c>
       <c r="D307">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E307">
         <v>49</v>
@@ -6192,7 +6192,7 @@
         <v>141</v>
       </c>
       <c r="D308">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E308">
         <v>46</v>
@@ -6209,7 +6209,7 @@
         <v>142</v>
       </c>
       <c r="D309">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E309">
         <v>59</v>
@@ -6226,7 +6226,7 @@
         <v>143</v>
       </c>
       <c r="D310">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E310">
         <v>41</v>
@@ -6243,7 +6243,7 @@
         <v>144</v>
       </c>
       <c r="D311">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E311">
         <v>42</v>
@@ -6277,7 +6277,7 @@
         <v>146</v>
       </c>
       <c r="D313">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E313">
         <v>72</v>
@@ -6294,7 +6294,7 @@
         <v>147</v>
       </c>
       <c r="D314">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E314">
         <v>149</v>
@@ -6311,7 +6311,7 @@
         <v>148</v>
       </c>
       <c r="D315">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E315">
         <v>185</v>
@@ -6328,7 +6328,7 @@
         <v>149</v>
       </c>
       <c r="D316">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E316">
         <v>172</v>
@@ -6345,7 +6345,7 @@
         <v>150</v>
       </c>
       <c r="D317">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E317">
         <v>143</v>
@@ -6362,7 +6362,7 @@
         <v>151</v>
       </c>
       <c r="D318">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E318">
         <v>104</v>
@@ -6379,7 +6379,7 @@
         <v>152</v>
       </c>
       <c r="D319">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E319">
         <v>52</v>
@@ -6396,7 +6396,7 @@
         <v>153</v>
       </c>
       <c r="D320">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E320">
         <v>39</v>
@@ -6413,7 +6413,7 @@
         <v>154</v>
       </c>
       <c r="D321">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E321">
         <v>36</v>
@@ -6430,7 +6430,7 @@
         <v>155</v>
       </c>
       <c r="D322">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E322">
         <v>34</v>
@@ -6447,7 +6447,7 @@
         <v>156</v>
       </c>
       <c r="D323">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E323">
         <v>50</v>
@@ -6464,7 +6464,7 @@
         <v>157</v>
       </c>
       <c r="D324">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E324">
         <v>48</v>
@@ -6481,7 +6481,7 @@
         <v>158</v>
       </c>
       <c r="D325">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E325">
         <v>39</v>
@@ -6498,7 +6498,7 @@
         <v>159</v>
       </c>
       <c r="D326">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E326">
         <v>49</v>
@@ -6515,7 +6515,7 @@
         <v>160</v>
       </c>
       <c r="D327">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E327">
         <v>45</v>
@@ -6532,7 +6532,7 @@
         <v>161</v>
       </c>
       <c r="D328">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E328">
         <v>38</v>
@@ -6549,7 +6549,7 @@
         <v>162</v>
       </c>
       <c r="D329">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E329">
         <v>72</v>
@@ -6566,7 +6566,7 @@
         <v>163</v>
       </c>
       <c r="D330">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E330">
         <v>88</v>
@@ -6583,7 +6583,7 @@
         <v>164</v>
       </c>
       <c r="D331">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E331">
         <v>52</v>
@@ -6617,7 +6617,7 @@
         <v>166</v>
       </c>
       <c r="D333">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E333">
         <v>54</v>
@@ -6668,7 +6668,7 @@
         <v>169</v>
       </c>
       <c r="D336">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E336">
         <v>82</v>
@@ -6685,7 +6685,7 @@
         <v>170</v>
       </c>
       <c r="D337">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E337">
         <v>180</v>
@@ -6719,7 +6719,7 @@
         <v>172</v>
       </c>
       <c r="D339">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E339">
         <v>97</v>
@@ -6753,7 +6753,7 @@
         <v>174</v>
       </c>
       <c r="D341">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E341">
         <v>50</v>
@@ -6770,7 +6770,7 @@
         <v>175</v>
       </c>
       <c r="D342">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E342">
         <v>58</v>
@@ -6872,7 +6872,7 @@
         <v>181</v>
       </c>
       <c r="D348">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E348">
         <v>58</v>
@@ -6906,7 +6906,7 @@
         <v>183</v>
       </c>
       <c r="D350">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E350">
         <v>60</v>
@@ -6940,7 +6940,7 @@
         <v>185</v>
       </c>
       <c r="D352">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E352">
         <v>65</v>
@@ -6957,7 +6957,7 @@
         <v>186</v>
       </c>
       <c r="D353">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E353">
         <v>182</v>
@@ -6974,7 +6974,7 @@
         <v>187</v>
       </c>
       <c r="D354">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E354">
         <v>238</v>
@@ -6991,7 +6991,7 @@
         <v>188</v>
       </c>
       <c r="D355">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E355">
         <v>94</v>
@@ -7096,7 +7096,7 @@
         <v>8</v>
       </c>
       <c r="E361">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="362" spans="1:5">
@@ -9580,7 +9580,7 @@
         <v>2</v>
       </c>
       <c r="E508">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="509" spans="1:5">
@@ -12589,7 +12589,7 @@
         <v>7</v>
       </c>
       <c r="E685">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="686" spans="1:5">
@@ -15561,10 +15561,10 @@
         <v>194</v>
       </c>
       <c r="D860">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E860">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="861" spans="1:5">
@@ -17587,7 +17587,7 @@
         <v>2</v>
       </c>
       <c r="E979">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="980" spans="1:5">
@@ -27192,10 +27192,10 @@
         <v>194</v>
       </c>
       <c r="D1577">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E1577">
-        <v>109</v>
+        <v>130</v>
       </c>
     </row>
     <row r="1578" spans="1:5">
@@ -30255,7 +30255,7 @@
         <v>2</v>
       </c>
       <c r="E1757">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1758" spans="1:5">
@@ -33312,10 +33312,10 @@
         <v>194</v>
       </c>
       <c r="D1937">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E1937">
-        <v>283</v>
+        <v>302</v>
       </c>
     </row>
     <row r="1938" spans="1:5">
@@ -36273,7 +36273,7 @@
         <v>5</v>
       </c>
       <c r="E2111">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2112" spans="1:5">

</xml_diff>